<commit_message>
add global architecture schema of bloc1 2 3
</commit_message>
<xml_diff>
--- a/Referentiel_master_RNCP/brouillon/brouillon Grille toutes les infos rassembler.xlsx
+++ b/Referentiel_master_RNCP/brouillon/brouillon Grille toutes les infos rassembler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Documents\Datapipeline_project_master\Referentiel_master_RNCP\brouillon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B302E-CAB5-49CD-874C-E0A3CF215594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185F7625-2C33-4127-A536-60F2B63D2EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
+    <workbookView xWindow="2895" yWindow="0" windowWidth="23955" windowHeight="15420" activeTab="2" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille Eval Bloc1" sheetId="2" r:id="rId1"/>
@@ -1606,35 +1606,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2280,7 +2280,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2986,7 +2986,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -4076,7 +4076,7 @@
       <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="70"/>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -4090,7 +4090,7 @@
       <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4137,9 +4137,9 @@
         <v>174</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="80"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="76"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4151,9 +4151,9 @@
         <v>175</v>
       </c>
       <c r="D9" s="38"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="77"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="73"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4165,9 +4165,9 @@
         <v>174</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="77"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="73"/>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4179,9 +4179,9 @@
         <v>174</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="73"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4193,9 +4193,9 @@
         <v>175</v>
       </c>
       <c r="D12" s="38"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="73"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4207,9 +4207,9 @@
         <v>174</v>
       </c>
       <c r="D13" s="38"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="77"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="73"/>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4221,9 +4221,9 @@
         <v>175</v>
       </c>
       <c r="D14" s="38"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="77"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="73"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4235,9 +4235,9 @@
         <v>175</v>
       </c>
       <c r="D15" s="38"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="77"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="73"/>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4249,9 +4249,9 @@
         <v>174</v>
       </c>
       <c r="D16" s="38"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="73"/>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4263,9 +4263,9 @@
         <v>174</v>
       </c>
       <c r="D17" s="36"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4279,9 +4279,9 @@
         <v>174</v>
       </c>
       <c r="D18" s="43"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="76"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4293,9 +4293,9 @@
         <v>175</v>
       </c>
       <c r="D19" s="47"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="73"/>
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4307,9 +4307,9 @@
         <v>175</v>
       </c>
       <c r="D20" s="47"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="73"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4321,9 +4321,9 @@
         <v>174</v>
       </c>
       <c r="D21" s="47"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="73"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4335,9 +4335,9 @@
         <v>175</v>
       </c>
       <c r="D22" s="47"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="73"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4349,9 +4349,9 @@
         <v>174</v>
       </c>
       <c r="D23" s="47"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="73"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4363,9 +4363,9 @@
         <v>174</v>
       </c>
       <c r="D24" s="47"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="73"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4377,9 +4377,9 @@
         <v>174</v>
       </c>
       <c r="D25" s="36"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="73"/>
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4393,9 +4393,9 @@
         <v>174</v>
       </c>
       <c r="D26" s="43"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="76"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4407,9 +4407,9 @@
         <v>175</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="77"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4421,9 +4421,9 @@
         <v>174</v>
       </c>
       <c r="D28" s="38"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="77"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="73"/>
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4435,9 +4435,9 @@
         <v>175</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="77"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="73"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" s="5" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4449,9 +4449,9 @@
         <v>175</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="77"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="73"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4463,9 +4463,9 @@
         <v>174</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="77"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="73"/>
       <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4477,9 +4477,9 @@
         <v>174</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="73"/>
       <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4491,9 +4491,9 @@
         <v>174</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="73"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4505,9 +4505,9 @@
         <v>174</v>
       </c>
       <c r="D34" s="38"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="77"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="73"/>
       <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" s="5" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4519,9 +4519,9 @@
         <v>174</v>
       </c>
       <c r="D35" s="36"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="77"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="73"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4535,9 +4535,9 @@
         <v>174</v>
       </c>
       <c r="D36" s="43"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="76"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="72"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4549,9 +4549,9 @@
         <v>174</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="77"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="73"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4563,9 +4563,9 @@
         <v>175</v>
       </c>
       <c r="D38" s="38"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="77"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="73"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4577,9 +4577,9 @@
         <v>175</v>
       </c>
       <c r="D39" s="38"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="77"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="73"/>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4591,9 +4591,9 @@
         <v>175</v>
       </c>
       <c r="D40" s="38"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="77"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="73"/>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4605,9 +4605,9 @@
         <v>174</v>
       </c>
       <c r="D41" s="38"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="77"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="73"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4619,9 +4619,9 @@
         <v>174</v>
       </c>
       <c r="D42" s="38"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="77"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="73"/>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4633,9 +4633,9 @@
         <v>174</v>
       </c>
       <c r="D43" s="38"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="77"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="73"/>
       <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4647,9 +4647,9 @@
         <v>174</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="77"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="73"/>
       <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4661,9 +4661,9 @@
         <v>174</v>
       </c>
       <c r="D45" s="48"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="77"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="73"/>
       <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4677,9 +4677,9 @@
         <v>174</v>
       </c>
       <c r="D46" s="43"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="76"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="72"/>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4691,9 +4691,9 @@
         <v>174</v>
       </c>
       <c r="D47" s="38"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="77"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="73"/>
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4705,9 +4705,9 @@
         <v>174</v>
       </c>
       <c r="D48" s="38"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="77"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="73"/>
       <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4719,9 +4719,9 @@
         <v>175</v>
       </c>
       <c r="D49" s="38"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="77"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="73"/>
       <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4733,9 +4733,9 @@
         <v>175</v>
       </c>
       <c r="D50" s="38"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="77"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="73"/>
       <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4747,9 +4747,9 @@
         <v>175</v>
       </c>
       <c r="D51" s="38"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="77"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="73"/>
       <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4761,9 +4761,9 @@
         <v>175</v>
       </c>
       <c r="D52" s="38"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="77"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="73"/>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4775,9 +4775,9 @@
         <v>174</v>
       </c>
       <c r="D53" s="38"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="77"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="73"/>
       <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4789,9 +4789,9 @@
         <v>174</v>
       </c>
       <c r="D54" s="38"/>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73"/>
-      <c r="G54" s="77"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="73"/>
       <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4803,9 +4803,9 @@
         <v>174</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="73"/>
-      <c r="F55" s="73"/>
-      <c r="G55" s="77"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="78"/>
+      <c r="G55" s="73"/>
       <c r="H55" s="9"/>
     </row>
     <row r="56" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4817,9 +4817,9 @@
         <v>174</v>
       </c>
       <c r="D56" s="36"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="78"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="81"/>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
@@ -4839,6 +4839,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F46:F56"/>
+    <mergeCell ref="E46:E56"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A46:A56"/>
+    <mergeCell ref="G46:G56"/>
+    <mergeCell ref="F26:F35"/>
+    <mergeCell ref="E26:E35"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="E36:E45"/>
+    <mergeCell ref="F36:F45"/>
+    <mergeCell ref="G36:G45"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:B4"/>
@@ -4854,17 +4865,6 @@
     <mergeCell ref="E8:E17"/>
     <mergeCell ref="F18:F25"/>
     <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F46:F56"/>
-    <mergeCell ref="E46:E56"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A46:A56"/>
-    <mergeCell ref="G46:G56"/>
-    <mergeCell ref="F26:F35"/>
-    <mergeCell ref="E26:E35"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="F36:F45"/>
-    <mergeCell ref="G36:G45"/>
   </mergeCells>
   <conditionalFormatting sqref="F58">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -4896,26 +4896,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097798227B93F3B46A4C8EE6693783472" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07a0dc2af2640077c1870da1684932dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ba08013-ef1c-4130-a497-bc53eb55e168" xmlns:ns3="0ed22885-9a1c-4a78-8ce9-dd4492997226" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f8b351a6a60032acdf3e22257ff17f6" ns2:_="" ns3:_="">
     <xsd:import namespace="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
@@ -5144,28 +5124,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
-    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
-    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
-    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B35CE1C-889F-46C7-9B5C-5C98D0751230}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5182,4 +5161,25 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
+    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
+    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
+    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
create dockerfile for deployement
</commit_message>
<xml_diff>
--- a/Referentiel_master_RNCP/brouillon/brouillon Grille toutes les infos rassembler.xlsx
+++ b/Referentiel_master_RNCP/brouillon/brouillon Grille toutes les infos rassembler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Documents\Datapipeline_project_master\Referentiel_master_RNCP\brouillon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185F7625-2C33-4127-A536-60F2B63D2EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318519F6-C04E-475D-AEED-1F339C4ED971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="0" windowWidth="23955" windowHeight="15420" activeTab="2" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
+    <workbookView xWindow="375" yWindow="75" windowWidth="27360" windowHeight="15180" activeTab="1" xr2:uid="{AB6F6693-6B8C-4684-9576-BC4DD09BE9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Grille Eval Bloc1" sheetId="2" r:id="rId1"/>
@@ -1606,35 +1606,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2280,7 +2280,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2651,7 +2651,7 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2868,7 +2868,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59"/>
       <c r="B14" s="17" t="s">
         <v>74</v>
@@ -2986,7 +2986,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -3344,7 +3344,7 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3675,7 +3675,7 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -4076,7 +4076,7 @@
       <c r="C4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="70"/>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -4090,7 +4090,7 @@
       <c r="C5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="74"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4137,9 +4137,9 @@
         <v>174</v>
       </c>
       <c r="D8" s="38"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="76"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4151,9 +4151,9 @@
         <v>175</v>
       </c>
       <c r="D9" s="38"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="77"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4165,9 +4165,9 @@
         <v>174</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4179,9 +4179,9 @@
         <v>174</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4193,9 +4193,9 @@
         <v>175</v>
       </c>
       <c r="D12" s="38"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="77"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4207,9 +4207,9 @@
         <v>174</v>
       </c>
       <c r="D13" s="38"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4221,9 +4221,9 @@
         <v>175</v>
       </c>
       <c r="D14" s="38"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4235,9 +4235,9 @@
         <v>175</v>
       </c>
       <c r="D15" s="38"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4249,9 +4249,9 @@
         <v>174</v>
       </c>
       <c r="D16" s="38"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="77"/>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4263,9 +4263,9 @@
         <v>174</v>
       </c>
       <c r="D17" s="36"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="77"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4279,9 +4279,9 @@
         <v>174</v>
       </c>
       <c r="D18" s="43"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="76"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4293,9 +4293,9 @@
         <v>175</v>
       </c>
       <c r="D19" s="47"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="77"/>
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4307,9 +4307,9 @@
         <v>175</v>
       </c>
       <c r="D20" s="47"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="77"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4321,9 +4321,9 @@
         <v>174</v>
       </c>
       <c r="D21" s="47"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4335,9 +4335,9 @@
         <v>175</v>
       </c>
       <c r="D22" s="47"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4349,9 +4349,9 @@
         <v>174</v>
       </c>
       <c r="D23" s="47"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4363,9 +4363,9 @@
         <v>174</v>
       </c>
       <c r="D24" s="47"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="77"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4377,9 +4377,9 @@
         <v>174</v>
       </c>
       <c r="D25" s="36"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="77"/>
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4393,9 +4393,9 @@
         <v>174</v>
       </c>
       <c r="D26" s="43"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="76"/>
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4407,9 +4407,9 @@
         <v>175</v>
       </c>
       <c r="D27" s="38"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="77"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4421,9 +4421,9 @@
         <v>174</v>
       </c>
       <c r="D28" s="38"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="77"/>
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -4435,9 +4435,9 @@
         <v>175</v>
       </c>
       <c r="D29" s="38"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="77"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" s="5" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4449,9 +4449,9 @@
         <v>175</v>
       </c>
       <c r="D30" s="38"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="77"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4463,9 +4463,9 @@
         <v>174</v>
       </c>
       <c r="D31" s="38"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="77"/>
       <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4477,9 +4477,9 @@
         <v>174</v>
       </c>
       <c r="D32" s="38"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="77"/>
       <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -4491,9 +4491,9 @@
         <v>174</v>
       </c>
       <c r="D33" s="38"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="73"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="77"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4505,9 +4505,9 @@
         <v>174</v>
       </c>
       <c r="D34" s="38"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="77"/>
       <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" s="5" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4519,9 +4519,9 @@
         <v>174</v>
       </c>
       <c r="D35" s="36"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="77"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" s="5" customFormat="1" ht="27.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4535,9 +4535,9 @@
         <v>174</v>
       </c>
       <c r="D36" s="43"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="76"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4549,9 +4549,9 @@
         <v>174</v>
       </c>
       <c r="D37" s="38"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="77"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4563,9 +4563,9 @@
         <v>175</v>
       </c>
       <c r="D38" s="38"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="77"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4577,9 +4577,9 @@
         <v>175</v>
       </c>
       <c r="D39" s="38"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="77"/>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4591,9 +4591,9 @@
         <v>175</v>
       </c>
       <c r="D40" s="38"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="77"/>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4605,9 +4605,9 @@
         <v>174</v>
       </c>
       <c r="D41" s="38"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="77"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4619,9 +4619,9 @@
         <v>174</v>
       </c>
       <c r="D42" s="38"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="77"/>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4633,9 +4633,9 @@
         <v>174</v>
       </c>
       <c r="D43" s="38"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="77"/>
       <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4647,9 +4647,9 @@
         <v>174</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="77"/>
       <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" s="5" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4661,9 +4661,9 @@
         <v>174</v>
       </c>
       <c r="D45" s="48"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="73"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="77"/>
       <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8" s="5" customFormat="1" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4677,9 +4677,9 @@
         <v>174</v>
       </c>
       <c r="D46" s="43"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="76"/>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4691,9 +4691,9 @@
         <v>174</v>
       </c>
       <c r="D47" s="38"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="73"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="77"/>
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4705,9 +4705,9 @@
         <v>174</v>
       </c>
       <c r="D48" s="38"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="73"/>
+      <c r="E48" s="73"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="77"/>
       <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4719,9 +4719,9 @@
         <v>175</v>
       </c>
       <c r="D49" s="38"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="73"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73"/>
+      <c r="G49" s="77"/>
       <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4733,9 +4733,9 @@
         <v>175</v>
       </c>
       <c r="D50" s="38"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
-      <c r="G50" s="73"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="77"/>
       <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4747,9 +4747,9 @@
         <v>175</v>
       </c>
       <c r="D51" s="38"/>
-      <c r="E51" s="78"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="77"/>
       <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4761,9 +4761,9 @@
         <v>175</v>
       </c>
       <c r="D52" s="38"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="73"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="77"/>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -4775,9 +4775,9 @@
         <v>174</v>
       </c>
       <c r="D53" s="38"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="73"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73"/>
+      <c r="G53" s="77"/>
       <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4789,9 +4789,9 @@
         <v>174</v>
       </c>
       <c r="D54" s="38"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="73"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="77"/>
       <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.25">
@@ -4803,9 +4803,9 @@
         <v>174</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
-      <c r="G55" s="73"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="77"/>
       <c r="H55" s="9"/>
     </row>
     <row r="56" spans="1:8" s="5" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4817,9 +4817,9 @@
         <v>174</v>
       </c>
       <c r="D56" s="36"/>
-      <c r="E56" s="80"/>
-      <c r="F56" s="80"/>
-      <c r="G56" s="81"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="78"/>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
@@ -4839,17 +4839,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F46:F56"/>
-    <mergeCell ref="E46:E56"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A46:A56"/>
-    <mergeCell ref="G46:G56"/>
-    <mergeCell ref="F26:F35"/>
-    <mergeCell ref="E26:E35"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="E36:E45"/>
-    <mergeCell ref="F36:F45"/>
-    <mergeCell ref="G36:G45"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:B4"/>
@@ -4865,6 +4854,17 @@
     <mergeCell ref="E8:E17"/>
     <mergeCell ref="F18:F25"/>
     <mergeCell ref="E18:E25"/>
+    <mergeCell ref="F46:F56"/>
+    <mergeCell ref="E46:E56"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A46:A56"/>
+    <mergeCell ref="G46:G56"/>
+    <mergeCell ref="F26:F35"/>
+    <mergeCell ref="E26:E35"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="E36:E45"/>
+    <mergeCell ref="F36:F45"/>
+    <mergeCell ref="G36:G45"/>
   </mergeCells>
   <conditionalFormatting sqref="F58">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -4896,6 +4896,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097798227B93F3B46A4C8EE6693783472" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="07a0dc2af2640077c1870da1684932dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ba08013-ef1c-4130-a497-bc53eb55e168" xmlns:ns3="0ed22885-9a1c-4a78-8ce9-dd4492997226" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f8b351a6a60032acdf3e22257ff17f6" ns2:_="" ns3:_="">
     <xsd:import namespace="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
@@ -5124,27 +5144,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
+    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
+    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
+    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ba08013-ef1c-4130-a497-bc53eb55e168" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ed22885-9a1c-4a78-8ce9-dd4492997226">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B35CE1C-889F-46C7-9B5C-5C98D0751230}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5161,25 +5182,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{801D0CEA-46D1-40C8-94B1-8478A557036E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6771D95-FB55-4106-9918-F95569952A80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81d943eb-53de-4d5a-93c5-961cb00f222e"/>
-    <ds:schemaRef ds:uri="11399b42-56c9-44ff-9016-8ae70501af32"/>
-    <ds:schemaRef ds:uri="1ba08013-ef1c-4130-a497-bc53eb55e168"/>
-    <ds:schemaRef ds:uri="0ed22885-9a1c-4a78-8ce9-dd4492997226"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>